<commit_message>
feat chart file added
</commit_message>
<xml_diff>
--- a/01_Spreadsheets_intro/01_Worksheets.xlsx.xlsx
+++ b/01_Spreadsheets_intro/01_Worksheets.xlsx.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91771\Desktop\data-analytics\excel\01_Spreadsheets_intro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C8A439-F866-4D1F-9ACC-3D71FD2E2C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B0BEE3-1DB4-4E63-9079-F5211C211FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -465,7 +468,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,6 +542,7 @@
       <c r="G6" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>